<commit_message>
added new data for OPM, CAVV and modify update date
</commit_message>
<xml_diff>
--- a/data/Negociado_de_Policia/npprDesp.xlsx
+++ b/data/Negociado_de_Policia/npprDesp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gnper\Documents\ViolenciaGeneroPR\data\Negociado_de_Policia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8686935-66A4-4CBA-AEEE-F1DE73CEEDDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96277E3-7E17-4058-AA31-5FAE2D6A573E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -326,7 +326,9 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -394,7 +396,7 @@
         <v>197</v>
       </c>
       <c r="J2" s="3">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -426,7 +428,7 @@
         <v>191</v>
       </c>
       <c r="J3" s="3">
-        <v>144</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -490,7 +492,7 @@
         <v>132</v>
       </c>
       <c r="J5" s="3">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -522,7 +524,7 @@
         <v>127</v>
       </c>
       <c r="J6" s="3">
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>